<commit_message>
example cv successfully produced
</commit_message>
<xml_diff>
--- a/2022-2023_Faculty_CVs.xlsx
+++ b/2022-2023_Faculty_CVs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mia/Desktop/auto_cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E85A954-196D-F84A-8F97-9CA897EC84BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B76330-041D-E043-825F-08B49BDC03E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,26 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Orcid</t>
-  </si>
-  <si>
-    <t>Marie Monfils</t>
-  </si>
-  <si>
-    <t>0000-0001-8971-6651</t>
-  </si>
-  <si>
-    <t>marie.monfils@utexas.edu</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -302,40 +283,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{853AF1F3-47C1-B641-9ADD-BBD4AF099A2F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>